<commit_message>
update spreadsheet file and final fixes for dotnet reader
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_FsSpreadsheet.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_FsSpreadsheet.xlsx
@@ -2,11 +2,44 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WithTable" sheetId="1" r:id="Rbedbae4e20e54521"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tableless" sheetId="2" r:id="Rc90254d72e4541ee"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WithTable_Duplicate" sheetId="3" r:id="R0e955896c6264149"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WithTable" sheetId="1" r:id="R7c2ffd854f1e4639"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tableless" sheetId="2" r:id="Ra99d3a677f6042cc"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WithTable_Duplicate" sheetId="3" r:id="Rf1829620e2844a84"/>
   </x:sheets>
 </x:workbook>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fonts count="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="1">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="22" fontId="0" fillId="0" borderId="0" applyNumberFormat="1"/>
+  </x:cellXfs>
+</x:styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,17 +96,17 @@
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6">
-      <x:c r="A2" t="e">
+      <x:c r="A2" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" t="str">
         <x:v>Hello</x:v>
       </x:c>
-      <x:c r="C2" t="e">
+      <x:c r="C2" s="1">
         <x:v>45213</x:v>
       </x:c>
       <x:c r="D2" t="b">
-        <x:v>1</x:v>
+        <x:v>true</x:v>
       </x:c>
       <x:c r="E2" t="str">
         <x:v>(A) This is part 1 of 2</x:v>
@@ -83,48 +116,48 @@
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
-      <x:c r="A3" t="e">
+      <x:c r="A3" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" t="str">
         <x:v>World</x:v>
       </x:c>
-      <x:c r="C3" t="e">
+      <x:c r="C3" s="2">
         <x:v>45214.75</x:v>
       </x:c>
       <x:c r="D3" t="b">
-        <x:v>0</x:v>
+        <x:v>false</x:v>
       </x:c>
       <x:c r="F3" t="str">
         <x:v>Tests if column names with whitespace at end can be unique</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
-      <x:c r="A4" t="e">
+      <x:c r="A4" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" t="str">
         <x:v>Bye</x:v>
       </x:c>
-      <x:c r="C4" t="e">
+      <x:c r="C4" s="2">
         <x:v>45215.833333333336</x:v>
       </x:c>
       <x:c r="D4" t="b">
-        <x:v>1</x:v>
+        <x:v>true</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
-      <x:c r="A5" t="e">
+      <x:c r="A5" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" t="str">
         <x:v>Outer Space</x:v>
       </x:c>
-      <x:c r="C5" t="e">
+      <x:c r="C5" s="1">
         <x:v>45216</x:v>
       </x:c>
       <x:c r="D5" t="b">
-        <x:v>0</x:v>
+        <x:v>false</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -158,17 +191,17 @@
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6">
-      <x:c r="A2" t="e">
+      <x:c r="A2" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" t="str">
         <x:v>Hello</x:v>
       </x:c>
-      <x:c r="C2" t="e">
+      <x:c r="C2" s="1">
         <x:v>45213</x:v>
       </x:c>
       <x:c r="D2" t="b">
-        <x:v>1</x:v>
+        <x:v>true</x:v>
       </x:c>
       <x:c r="E2" t="str">
         <x:v>(A) This is part 1 of 2</x:v>
@@ -178,48 +211,48 @@
       </x:c>
     </x:row>
     <x:row r="3" spans="1:6">
-      <x:c r="A3" t="e">
+      <x:c r="A3" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" t="str">
         <x:v>World</x:v>
       </x:c>
-      <x:c r="C3" t="e">
+      <x:c r="C3" s="2">
         <x:v>45214.75</x:v>
       </x:c>
       <x:c r="D3" t="b">
-        <x:v>0</x:v>
+        <x:v>false</x:v>
       </x:c>
       <x:c r="F3" t="str">
         <x:v>Tests if column names with whitespace at end can be unique</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
-      <x:c r="A4" t="e">
+      <x:c r="A4" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" t="str">
         <x:v>Bye</x:v>
       </x:c>
-      <x:c r="C4" t="e">
+      <x:c r="C4" s="2">
         <x:v>45215.833333333336</x:v>
       </x:c>
       <x:c r="D4" t="b">
-        <x:v>1</x:v>
+        <x:v>true</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
-      <x:c r="A5" t="e">
+      <x:c r="A5" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" t="str">
         <x:v>Outer Space</x:v>
       </x:c>
-      <x:c r="C5" t="e">
+      <x:c r="C5" s="1">
         <x:v>45216</x:v>
       </x:c>
       <x:c r="D5" t="b">
-        <x:v>0</x:v>
+        <x:v>false</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -250,17 +283,17 @@
       </x:c>
     </x:row>
     <x:row r="5" spans="2:7">
-      <x:c r="B5" t="e">
+      <x:c r="B5" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="C5" t="str">
         <x:v>Hello</x:v>
       </x:c>
-      <x:c r="D5" t="e">
+      <x:c r="D5" s="1">
         <x:v>45213</x:v>
       </x:c>
       <x:c r="E5" t="b">
-        <x:v>1</x:v>
+        <x:v>true</x:v>
       </x:c>
       <x:c r="F5" t="str">
         <x:v>(A) This is part 1 of 2</x:v>
@@ -270,48 +303,48 @@
       </x:c>
     </x:row>
     <x:row r="6" spans="2:7">
-      <x:c r="B6" t="e">
+      <x:c r="B6" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="C6" t="str">
         <x:v>World</x:v>
       </x:c>
-      <x:c r="D6" t="e">
+      <x:c r="D6" s="2">
         <x:v>45214.75</x:v>
       </x:c>
       <x:c r="E6" t="b">
-        <x:v>0</x:v>
+        <x:v>false</x:v>
       </x:c>
       <x:c r="G6" t="str">
         <x:v>Tests if column names with whitespace at end can be unique</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:5">
-      <x:c r="B7" t="e">
+      <x:c r="B7" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C7" t="str">
         <x:v>Bye</x:v>
       </x:c>
-      <x:c r="D7" t="e">
+      <x:c r="D7" s="2">
         <x:v>45215.833333333336</x:v>
       </x:c>
       <x:c r="E7" t="b">
-        <x:v>1</x:v>
+        <x:v>true</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5">
-      <x:c r="B8" t="e">
+      <x:c r="B8" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="C8" t="str">
         <x:v>Outer Space</x:v>
       </x:c>
-      <x:c r="D8" t="e">
+      <x:c r="D8" s="1">
         <x:v>45216</x:v>
       </x:c>
       <x:c r="E8" t="b">
-        <x:v>0</x:v>
+        <x:v>false</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Further work on #71 change FsCell.Value to obj :boom:
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_FsSpreadsheet.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_FsSpreadsheet.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WithTable" sheetId="1" r:id="Ra18693de6f3e45fd"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tableless" sheetId="2" r:id="Ra6d38832c9ff4312"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WithTable_Duplicate" sheetId="3" r:id="R8efa0ef73b884f5d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WithTable" sheetId="1" r:id="R71d39628c6ae4ef0"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tableless" sheetId="2" r:id="Rf21e7a5520544f5e"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WithTable_Duplicate" sheetId="3" r:id="R5fb9c0bcbccc494f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -106,7 +106,7 @@
         <x:v>45213</x:v>
       </x:c>
       <x:c r="D2" t="b">
-        <x:v>true</x:v>
+        <x:v>True</x:v>
       </x:c>
       <x:c r="E2" t="str">
         <x:v>(A) This is part 1 of 2</x:v>
@@ -126,7 +126,7 @@
         <x:v>45214.75</x:v>
       </x:c>
       <x:c r="D3" t="b">
-        <x:v>false</x:v>
+        <x:v>False</x:v>
       </x:c>
       <x:c r="F3" t="str">
         <x:v>Tests if column names with whitespace at end can be unique</x:v>
@@ -143,7 +143,7 @@
         <x:v>45215.833333333336</x:v>
       </x:c>
       <x:c r="D4" t="b">
-        <x:v>true</x:v>
+        <x:v>True</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -157,7 +157,7 @@
         <x:v>45216</x:v>
       </x:c>
       <x:c r="D5" t="b">
-        <x:v>false</x:v>
+        <x:v>False</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -201,7 +201,7 @@
         <x:v>45213</x:v>
       </x:c>
       <x:c r="D2" t="b">
-        <x:v>true</x:v>
+        <x:v>True</x:v>
       </x:c>
       <x:c r="E2" t="str">
         <x:v>(A) This is part 1 of 2</x:v>
@@ -221,7 +221,7 @@
         <x:v>45214.75</x:v>
       </x:c>
       <x:c r="D3" t="b">
-        <x:v>false</x:v>
+        <x:v>False</x:v>
       </x:c>
       <x:c r="F3" t="str">
         <x:v>Tests if column names with whitespace at end can be unique</x:v>
@@ -238,7 +238,7 @@
         <x:v>45215.833333333336</x:v>
       </x:c>
       <x:c r="D4" t="b">
-        <x:v>true</x:v>
+        <x:v>True</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:4">
@@ -252,7 +252,7 @@
         <x:v>45216</x:v>
       </x:c>
       <x:c r="D5" t="b">
-        <x:v>false</x:v>
+        <x:v>False</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -293,7 +293,7 @@
         <x:v>45213</x:v>
       </x:c>
       <x:c r="E5" t="b">
-        <x:v>true</x:v>
+        <x:v>True</x:v>
       </x:c>
       <x:c r="F5" t="str">
         <x:v>(A) This is part 1 of 2</x:v>
@@ -313,7 +313,7 @@
         <x:v>45214.75</x:v>
       </x:c>
       <x:c r="E6" t="b">
-        <x:v>false</x:v>
+        <x:v>False</x:v>
       </x:c>
       <x:c r="G6" t="str">
         <x:v>Tests if column names with whitespace at end can be unique</x:v>
@@ -330,7 +330,7 @@
         <x:v>45215.833333333336</x:v>
       </x:c>
       <x:c r="E7" t="b">
-        <x:v>true</x:v>
+        <x:v>True</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="2:5">
@@ -344,7 +344,7 @@
         <x:v>45216</x:v>
       </x:c>
       <x:c r="E8" t="b">
-        <x:v>false</x:v>
+        <x:v>False</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>